<commit_message>
Remove all references from API
</commit_message>
<xml_diff>
--- a/docs/source/index/tables/0_mapper.xlsx
+++ b/docs/source/index/tables/0_mapper.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">See also</t>
+    <t xml:space="preserve">See Also</t>
   </si>
   <si>
     <t xml:space="preserve">1_overview_benchmarks</t>
@@ -170,10 +170,10 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>

</xml_diff>